<commit_message>
update becf, etle, ets
</commit_message>
<xml_diff>
--- a/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
+++ b/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\ETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738849F8-3EF3-4804-8F67-3336470FA6D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C908A8B1-F2BC-451A-A817-67326C7F17A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="645" yWindow="660" windowWidth="24975" windowHeight="16290" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="ETS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422D012-50FD-4D0C-A3BE-19778A6AC198}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -689,8 +689,8 @@
   </sheetPr>
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,97 +1193,97 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AF6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -1291,97 +1291,97 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates to ETS to revert to 1 for better balance in deep decarbonizatoin scenarios and updates to subsidies to reflect CA-specific capital costs
</commit_message>
<xml_diff>
--- a/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
+++ b/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\ETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\ETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C908A8B1-F2BC-451A-A817-67326C7F17A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77477890-FFCA-46B3-8D29-E14C8769BDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="660" windowWidth="24975" windowHeight="16290" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -690,7 +690,7 @@
   <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6:AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,97 +1193,97 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="X6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AD6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -1291,97 +1291,97 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set shareweight to 0 for MSW
</commit_message>
<xml_diff>
--- a/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
+++ b/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\ETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77477890-FFCA-46B3-8D29-E14C8769BDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFC4F3C-0127-4097-A9A6-7DC1F58CFD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
@@ -690,7 +690,7 @@
   <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:AF7"/>
+      <selection activeCell="B17" sqref="B17:AF17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,97 +2271,97 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>